<commit_message>
added progress report on DeePromoter dataset.
</commit_message>
<xml_diff>
--- a/recap-2.xlsx
+++ b/recap-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Reference\research\sequence-processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA9EC19-4944-4548-978C-143937C41568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA7833A-3A4E-4572-B56E-8D200D86D1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3330" yWindow="-15030" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{ADCB0F8D-F952-422A-A60B-628E8E9D1690}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
   <si>
     <t>metrics</t>
   </si>
@@ -135,6 +135,9 @@
   <si>
     <t>TATA Promoter</t>
   </si>
+  <si>
+    <t>CCAAT Promoter</t>
+  </si>
 </sst>
 </file>
 
@@ -213,11 +216,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -1486,7 +1489,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-ID"/>
-              <a:t>Prediksi TATA Promoter dari Dataset Human Genome GrCh38</a:t>
+              <a:t>Prediksi TATA Promoter dari Dataset Human Genome GrCh38 (Pre-Fine Tuning)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2007,6 +2010,567 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-ID"/>
+              <a:t>Prediksi CCAAT Promoter pada Genom</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-ID" baseline="0"/>
+              <a:t> Manusia dari Dataset GRCh37 (Pre-Fine Tuning)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-ID"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'15082021'!$C$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>k-mer 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'15082021'!$B$18:$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>acc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>f1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>precision</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>recall</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'15082021'!$C$18:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.55102040816326503</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52237483385024297</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56712328767123199</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55102040816326503</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9327-4863-B03E-125C4BBE2612}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'15082021'!$D$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>k-mer 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'15082021'!$B$18:$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>acc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>f1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>precision</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>recall</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'15082021'!$D$18:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.57142857142857095</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56981605351170495</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.57251585623678602</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.57142857142857095</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9327-4863-B03E-125C4BBE2612}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'15082021'!$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>k-mer 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'15082021'!$B$18:$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>acc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>f1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>precision</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>recall</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'15082021'!$E$18:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.52040816326530603</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.467083188707624</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53402777777777699</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.52040816326530603</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9327-4863-B03E-125C4BBE2612}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'15082021'!$F$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>k-mer 6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'15082021'!$B$18:$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>acc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>f1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>precision</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>recall</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'15082021'!$F$18:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.42857142857142799</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.38530465949820702</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.40057971014492699</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42857142857142799</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9327-4863-B03E-125C4BBE2612}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="98108191"/>
+        <c:axId val="98114431"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="98108191"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="98114431"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="98114431"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="98108191"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2127,6 +2691,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
@@ -3125,6 +3729,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3673,15 +4780,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3708,16 +4815,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>395287</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>90487</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3737,6 +4844,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDD583C8-7E02-4031-9BDF-C99BC250A427}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4071,7 +5214,7 @@
       </c>
     </row>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D3" t="s">
@@ -4091,7 +5234,7 @@
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="4"/>
+      <c r="C4" s="6"/>
       <c r="D4" t="s">
         <v>2</v>
       </c>
@@ -4109,7 +5252,7 @@
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="4"/>
+      <c r="C5" s="6"/>
       <c r="D5" t="s">
         <v>3</v>
       </c>
@@ -4127,7 +5270,7 @@
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="4"/>
+      <c r="C6" s="6"/>
       <c r="D6" t="s">
         <v>4</v>
       </c>
@@ -4145,7 +5288,7 @@
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="4"/>
+      <c r="C7" s="6"/>
       <c r="D7" t="s">
         <v>5</v>
       </c>
@@ -4163,7 +5306,7 @@
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="4"/>
+      <c r="C8" s="6"/>
       <c r="D8" t="s">
         <v>6</v>
       </c>
@@ -4225,7 +5368,7 @@
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D15" t="s">
@@ -4245,7 +5388,7 @@
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="4"/>
+      <c r="C16" s="6"/>
       <c r="D16" t="s">
         <v>2</v>
       </c>
@@ -4263,7 +5406,7 @@
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="4"/>
+      <c r="C17" s="6"/>
       <c r="D17" t="s">
         <v>3</v>
       </c>
@@ -4281,7 +5424,7 @@
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="4"/>
+      <c r="C18" s="6"/>
       <c r="D18" t="s">
         <v>4</v>
       </c>
@@ -4299,7 +5442,7 @@
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="4"/>
+      <c r="C19" s="6"/>
       <c r="D19" t="s">
         <v>5</v>
       </c>
@@ -4317,7 +5460,7 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="4"/>
+      <c r="C20" s="6"/>
       <c r="D20" t="s">
         <v>6</v>
       </c>
@@ -4347,15 +5490,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB076EBC-2ACD-4CAD-97E6-A437874FFD9F}">
-  <dimension ref="B2:F14"/>
+  <dimension ref="B2:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
@@ -4364,85 +5507,85 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>0.46666666666666601</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>0.18666666666666601</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>0.37333333333333302</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>0.43333333333333302</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>0.36886741814278001</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>0.188096744073973</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>0.296777725858903</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>0.39721374554252398</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>0.30708898944193003</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>0.190749173307312</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>0.39623507805325903</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>0.43507371135092399</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>0.46666666666666601</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>0.18666666666666601</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>0.37333333333333302</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>0.43333333333333302</v>
       </c>
     </row>
@@ -4452,85 +5595,184 @@
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>0.51020408163265296</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>0.38775510204081598</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>0.56122448979591799</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>0.54081632653061196</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>0.57809246147438498</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>0.375</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>0.51911445851877203</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>0.49674768914755202</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>0.51342465753424604</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>0.37777777777777699</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>0.59423076923076901</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>0.56282051282051204</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>0.51020408163265296</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>0.38775510204081598</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>0.56122448979591799</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>0.54081632653061196</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f>AVERAGE(C11:C14)</f>
+        <v>0.52798132056848424</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.55102040816326503</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.52040816326530603</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.42857142857142799</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.52237483385024297</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.56981605351170495</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.467083188707624</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.38530465949820702</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.56712328767123199</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.57251585623678602</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.53402777777777699</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.40057971014492699</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.55102040816326503</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.52040816326530603</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0.42857142857142799</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <f>AVERAGE(C18:C21)</f>
+        <v>0.54788473446200125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added deepromoter setup files.
</commit_message>
<xml_diff>
--- a/recap-2.xlsx
+++ b/recap-2.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Reference\research\sequence-processing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\research\sequence-processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA7833A-3A4E-4572-B56E-8D200D86D1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA988AB-F2DA-43A2-8290-FD2577F79754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3330" yWindow="-15030" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{ADCB0F8D-F952-422A-A60B-628E8E9D1690}"/>
+    <workbookView xWindow="-2040" yWindow="-15990" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{ADCB0F8D-F952-422A-A60B-628E8E9D1690}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="15082021" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
   <si>
     <t>metrics</t>
   </si>
@@ -138,6 +139,24 @@
   <si>
     <t>CCAAT Promoter</t>
   </si>
+  <si>
+    <t>human_tata_positive</t>
+  </si>
+  <si>
+    <t>human_tata_negative</t>
+  </si>
+  <si>
+    <t>macaca_tata_positive</t>
+  </si>
+  <si>
+    <t>macaca_tata_negative</t>
+  </si>
+  <si>
+    <t>TATA Prediction</t>
+  </si>
+  <si>
+    <t>Non TATA Prediction</t>
+  </si>
 </sst>
 </file>
 
@@ -146,7 +165,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +176,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -211,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -220,6 +246,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2571,6 +2603,519 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-ID"/>
+              <a:t>Performa Akurasi Model TATA &amp; Non TATA pada</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-ID" baseline="0"/>
+              <a:t> Dataset Manusia dan Macaca</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-ID"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>human_tata_positive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$C$2:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>TATA Prediction</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Non TATA Prediction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$3:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="0.00%">
+                  <c:v>0.52600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E47A-42EF-B786-6C7B3B1C2113}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>human_tata_negative</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$C$2:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>TATA Prediction</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Non TATA Prediction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$4:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="0.00%">
+                  <c:v>0.54300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E47A-42EF-B786-6C7B3B1C2113}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>macaca_tata_positive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$C$2:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>TATA Prediction</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Non TATA Prediction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$5:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.44669999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19670000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E47A-42EF-B786-6C7B3B1C2113}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>macaca_tata_negative</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$C$2:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>TATA Prediction</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Non TATA Prediction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$6:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="0%">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28670000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E47A-42EF-B786-6C7B3B1C2113}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1390412192"/>
+        <c:axId val="1390424672"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1390412192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1390424672"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1390424672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1390412192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2731,6 +3276,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
@@ -4232,6 +4817,509 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4888,6 +5976,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3703D3B0-4CA2-44E3-9392-DC9AA0907D31}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5492,7 +6621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB076EBC-2ACD-4CAD-97E6-A437874FFD9F}">
   <dimension ref="B2:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -5779,4 +6908,78 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5DE264-5DA1-4264-91B3-8E16BC9637DE}">
+  <dimension ref="B2:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.44669999999999999</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.19670000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.28670000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>